<commit_message>
Power and Polarization Cal
</commit_message>
<xml_diff>
--- a/calibration records/Power Calibration Log.xlsx
+++ b/calibration records/Power Calibration Log.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ozymandias\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ozymandias\qudi-Purdue-modules\calibration records\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4114DD1-7B51-44D2-BF3E-847422AF76F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BFA9BC1-1945-4AB3-9970-CF5F58E9EB27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{27264247-0BF4-48CD-8C04-3DC7F13F065F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{27264247-0BF4-48CD-8C04-3DC7F13F065F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="15">
   <si>
     <t>Calibration Date</t>
   </si>
@@ -72,6 +72,15 @@
   </si>
   <si>
     <t>Polarization Power Ratio (expect ~1000:1)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10mW </t>
+  </si>
+  <si>
+    <t>Config File Updated?</t>
+  </si>
+  <si>
+    <t>Y</t>
   </si>
 </sst>
 </file>
@@ -107,9 +116,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -444,10 +454,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90E69C1E-AA36-4167-9E80-702D6744EA5A}">
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -457,13 +467,14 @@
     <col min="3" max="3" width="31" customWidth="1"/>
     <col min="4" max="4" width="19.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15.42578125" customWidth="1"/>
-    <col min="6" max="6" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24" customWidth="1"/>
     <col min="7" max="7" width="20" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="38" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15" customWidth="1"/>
+    <col min="9" max="9" width="38" customWidth="1"/>
+    <col min="10" max="10" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -489,10 +500,13 @@
         <v>11</v>
       </c>
       <c r="I1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>45635</v>
       </c>
@@ -520,15 +534,18 @@
         <v>1243.3333333333335</v>
       </c>
       <c r="I2" t="s">
+        <v>14</v>
+      </c>
+      <c r="J2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>45751</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="C3">
         <v>691</v>
@@ -551,6 +568,43 @@
         <v>950.53763440860212</v>
       </c>
       <c r="I3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>45890</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4">
+        <v>910</v>
+      </c>
+      <c r="D4">
+        <v>8210</v>
+      </c>
+      <c r="E4">
+        <f>D4/C4</f>
+        <v>9.0219780219780219</v>
+      </c>
+      <c r="F4" s="2">
+        <v>30000</v>
+      </c>
+      <c r="G4">
+        <v>30.3</v>
+      </c>
+      <c r="H4">
+        <f>F4/G4</f>
+        <v>990.09900990099004</v>
+      </c>
+      <c r="I4" t="s">
+        <v>14</v>
+      </c>
+      <c r="J4" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>